<commit_message>
Report of results for 3 configurations. 1.xml is very promising, but times are a bit too large.
</commit_message>
<xml_diff>
--- a/L1/Test 2711 - OttaM/ResAnalysis 2711.xlsx
+++ b/L1/Test 2711 - OttaM/ResAnalysis 2711.xlsx
@@ -11,7 +11,7 @@
   </sheets>
   <calcPr calcId="124519"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId2"/>
+    <pivotCache cacheId="0" r:id="rId2"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -170,7 +170,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,7 +186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -198,8 +205,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -207,11 +220,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -226,9 +260,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -2957,7 +2996,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot4" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori Minimi" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori Minimi" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="F1:I36" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -3645,7 +3684,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori Medi" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabella_pivot3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valori Medi" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:D36" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -4579,10 +4618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4597,7 +4636,7 @@
     <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:18">
       <c r="B1" s="3" t="s">
         <v>35</v>
       </c>
@@ -4605,7 +4644,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:18">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -4631,7 +4670,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -4644,6 +4683,9 @@
       <c r="D3" s="2">
         <v>10</v>
       </c>
+      <c r="E3" s="8">
+        <v>827.3</v>
+      </c>
       <c r="F3" s="1" t="s">
         <v>1</v>
       </c>
@@ -4656,8 +4698,12 @@
       <c r="I3" s="2">
         <v>10</v>
       </c>
+      <c r="R3" s="11">
+        <f>(B3-E3)/E3</f>
+        <v>1.9823522301466549E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:18">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -4670,6 +4716,9 @@
       <c r="D4" s="2">
         <v>10</v>
       </c>
+      <c r="E4" s="9">
+        <v>827.3</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>2</v>
       </c>
@@ -4682,8 +4731,12 @@
       <c r="I4" s="2">
         <v>10</v>
       </c>
+      <c r="R4" s="11">
+        <f t="shared" ref="R4:R35" si="0">(B4-E4)/E4</f>
+        <v>6.297594584794227E-3</v>
+      </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:18">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -4696,6 +4749,9 @@
       <c r="D5" s="2">
         <v>10</v>
       </c>
+      <c r="E5" s="10">
+        <v>826.3</v>
+      </c>
       <c r="F5" s="1" t="s">
         <v>3</v>
       </c>
@@ -4708,8 +4764,12 @@
       <c r="I5" s="2">
         <v>10</v>
       </c>
+      <c r="R5" s="11">
+        <f t="shared" si="0"/>
+        <v>3.4826334261164146E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:18">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -4722,6 +4782,9 @@
       <c r="D6" s="2">
         <v>10</v>
       </c>
+      <c r="E6" s="9">
+        <v>822.9</v>
+      </c>
       <c r="F6" s="1" t="s">
         <v>4</v>
       </c>
@@ -4734,8 +4797,12 @@
       <c r="I6" s="2">
         <v>10</v>
       </c>
+      <c r="R6" s="11">
+        <f t="shared" si="0"/>
+        <v>5.1794871794871744E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:18">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -4748,6 +4815,9 @@
       <c r="D7" s="2">
         <v>10</v>
       </c>
+      <c r="E7" s="10">
+        <v>827.3</v>
+      </c>
       <c r="F7" s="1" t="s">
         <v>5</v>
       </c>
@@ -4760,8 +4830,12 @@
       <c r="I7" s="2">
         <v>10</v>
       </c>
+      <c r="R7" s="11">
+        <f t="shared" si="0"/>
+        <v>1.9823522301466549E-3</v>
+      </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:18">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -4774,6 +4848,9 @@
       <c r="D8" s="2">
         <v>10.1</v>
       </c>
+      <c r="E8" s="9">
+        <v>827.3</v>
+      </c>
       <c r="F8" s="1" t="s">
         <v>6</v>
       </c>
@@ -4786,8 +4863,12 @@
       <c r="I8" s="2">
         <v>10</v>
       </c>
+      <c r="R8" s="11">
+        <f t="shared" si="0"/>
+        <v>1.49184092832107E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:18">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -4800,6 +4881,9 @@
       <c r="D9" s="2">
         <v>10</v>
       </c>
+      <c r="E9" s="10">
+        <v>827.3</v>
+      </c>
       <c r="F9" s="1" t="s">
         <v>7</v>
       </c>
@@ -4812,8 +4896,12 @@
       <c r="I9" s="2">
         <v>10</v>
       </c>
+      <c r="R9" s="11">
+        <f t="shared" si="0"/>
+        <v>1.4797534147226009E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:18">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -4826,6 +4914,9 @@
       <c r="D10" s="2">
         <v>10.199999999999999</v>
       </c>
+      <c r="E10" s="9">
+        <v>827.3</v>
+      </c>
       <c r="F10" s="1" t="s">
         <v>8</v>
       </c>
@@ -4838,8 +4929,12 @@
       <c r="I10" s="2">
         <v>10</v>
       </c>
+      <c r="R10" s="11">
+        <f t="shared" si="0"/>
+        <v>1.7040976671098978E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:18">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -4852,6 +4947,9 @@
       <c r="D11" s="2">
         <v>10</v>
       </c>
+      <c r="E11" s="10">
+        <v>827.3</v>
+      </c>
       <c r="F11" s="1" t="s">
         <v>9</v>
       </c>
@@ -4864,8 +4962,12 @@
       <c r="I11" s="2">
         <v>10</v>
       </c>
+      <c r="R11" s="11">
+        <f t="shared" si="0"/>
+        <v>5.1057657439869302E-3</v>
+      </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:18">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -4878,6 +4980,9 @@
       <c r="D12" s="2">
         <v>3</v>
       </c>
+      <c r="E12" s="9">
+        <v>589.1</v>
+      </c>
       <c r="F12" s="1" t="s">
         <v>10</v>
       </c>
@@ -4890,8 +4995,12 @@
       <c r="I12" s="2">
         <v>3</v>
       </c>
+      <c r="R12" s="11">
+        <f t="shared" si="0"/>
+        <v>4.1758614836187556E-3</v>
+      </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:18">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -4904,6 +5013,9 @@
       <c r="D13" s="2">
         <v>3</v>
       </c>
+      <c r="E13" s="10">
+        <v>589.1</v>
+      </c>
       <c r="F13" s="1" t="s">
         <v>11</v>
       </c>
@@ -4916,8 +5028,12 @@
       <c r="I13" s="2">
         <v>3</v>
       </c>
+      <c r="R13" s="11">
+        <f t="shared" si="0"/>
+        <v>4.1758614836187556E-3</v>
+      </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:18">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -4930,6 +5046,9 @@
       <c r="D14" s="2">
         <v>3</v>
       </c>
+      <c r="E14" s="9">
+        <v>588.70000000000005</v>
+      </c>
       <c r="F14" s="1" t="s">
         <v>12</v>
       </c>
@@ -4942,8 +5061,12 @@
       <c r="I14" s="2">
         <v>3</v>
       </c>
+      <c r="R14" s="11">
+        <f t="shared" si="0"/>
+        <v>1.0338032953966387E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:18">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -4956,6 +5079,9 @@
       <c r="D15" s="2">
         <v>3</v>
       </c>
+      <c r="E15" s="10">
+        <v>588.1</v>
+      </c>
       <c r="F15" s="1" t="s">
         <v>13</v>
       </c>
@@ -4968,8 +5094,12 @@
       <c r="I15" s="2">
         <v>3</v>
       </c>
+      <c r="R15" s="11">
+        <f t="shared" si="0"/>
+        <v>1.0476109505186291E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:18">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -4982,6 +5112,9 @@
       <c r="D16" s="2">
         <v>3</v>
       </c>
+      <c r="E16" s="9">
+        <v>586.4</v>
+      </c>
       <c r="F16" s="1" t="s">
         <v>14</v>
       </c>
@@ -4994,8 +5127,12 @@
       <c r="I16" s="2">
         <v>3</v>
       </c>
+      <c r="R16" s="11">
+        <f t="shared" si="0"/>
+        <v>4.2291950886767021E-3</v>
+      </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:18">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -5008,6 +5145,9 @@
       <c r="D17" s="2">
         <v>3</v>
       </c>
+      <c r="E17" s="10">
+        <v>586</v>
+      </c>
       <c r="F17" s="1" t="s">
         <v>15</v>
       </c>
@@ -5020,8 +5160,12 @@
       <c r="I17" s="2">
         <v>3</v>
       </c>
+      <c r="R17" s="11">
+        <f t="shared" si="0"/>
+        <v>4.2491467576790025E-3</v>
+      </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:18">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -5034,6 +5178,9 @@
       <c r="D18" s="2">
         <v>3</v>
       </c>
+      <c r="E18" s="9">
+        <v>585.79999999999995</v>
+      </c>
       <c r="F18" s="1" t="s">
         <v>16</v>
       </c>
@@ -5046,8 +5193,12 @@
       <c r="I18" s="2">
         <v>3</v>
       </c>
+      <c r="R18" s="11">
+        <f t="shared" si="0"/>
+        <v>4.2505974735404734E-3</v>
+      </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:18">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -5060,6 +5211,9 @@
       <c r="D19" s="2">
         <v>3</v>
       </c>
+      <c r="E19" s="10">
+        <v>585.79999999999995</v>
+      </c>
       <c r="F19" s="1" t="s">
         <v>17</v>
       </c>
@@ -5072,8 +5226,12 @@
       <c r="I19" s="2">
         <v>3</v>
       </c>
+      <c r="R19" s="11">
+        <f t="shared" si="0"/>
+        <v>4.3018094912939259E-3</v>
+      </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:18">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -5086,6 +5244,9 @@
       <c r="D20" s="2">
         <v>16.399999999999999</v>
       </c>
+      <c r="E20" s="9">
+        <v>1619.8</v>
+      </c>
       <c r="F20" s="1" t="s">
         <v>18</v>
       </c>
@@ -5098,8 +5259,12 @@
       <c r="I20" s="2">
         <v>16</v>
       </c>
+      <c r="R20" s="11">
+        <f t="shared" si="0"/>
+        <v>3.1021731077911008E-2</v>
+      </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:18">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -5112,6 +5277,9 @@
       <c r="D21" s="2">
         <v>14.9</v>
       </c>
+      <c r="E21" s="10">
+        <v>1457.4</v>
+      </c>
       <c r="F21" s="1" t="s">
         <v>19</v>
       </c>
@@ -5124,8 +5292,12 @@
       <c r="I21" s="2">
         <v>14</v>
       </c>
+      <c r="R21" s="11">
+        <f t="shared" si="0"/>
+        <v>3.1852614244545094E-2</v>
+      </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:18">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -5138,6 +5310,9 @@
       <c r="D22" s="2">
         <v>12.4</v>
       </c>
+      <c r="E22" s="9">
+        <v>1258</v>
+      </c>
       <c r="F22" s="6" t="s">
         <v>20</v>
       </c>
@@ -5153,8 +5328,12 @@
       <c r="J22" t="s">
         <v>43</v>
       </c>
+      <c r="R22" s="11">
+        <f t="shared" si="0"/>
+        <v>7.2453895071542262E-2</v>
+      </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:18">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -5167,6 +5346,9 @@
       <c r="D23" s="2">
         <v>11</v>
       </c>
+      <c r="E23" s="10">
+        <v>1132.3</v>
+      </c>
       <c r="F23" s="1" t="s">
         <v>21</v>
       </c>
@@ -5179,8 +5361,12 @@
       <c r="I23" s="2">
         <v>10</v>
       </c>
+      <c r="R23" s="11">
+        <f t="shared" si="0"/>
+        <v>5.8729135388148043E-2</v>
+      </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:18">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -5193,6 +5379,9 @@
       <c r="D24" s="2">
         <v>15.9</v>
       </c>
+      <c r="E24" s="9">
+        <v>1513.7</v>
+      </c>
       <c r="F24" s="1" t="s">
         <v>22</v>
       </c>
@@ -5205,8 +5394,12 @@
       <c r="I24" s="2">
         <v>15</v>
       </c>
+      <c r="R24" s="11">
+        <f t="shared" si="0"/>
+        <v>3.4909823611019408E-2</v>
+      </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:18">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -5219,6 +5412,9 @@
       <c r="D25" s="2">
         <v>13.7</v>
       </c>
+      <c r="E25" s="10">
+        <v>1372.7</v>
+      </c>
       <c r="F25" s="1" t="s">
         <v>23</v>
       </c>
@@ -5231,8 +5427,12 @@
       <c r="I25" s="2">
         <v>13</v>
       </c>
+      <c r="R25" s="11">
+        <f t="shared" si="0"/>
+        <v>3.5607197493989891E-2</v>
+      </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:18">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -5245,6 +5445,9 @@
       <c r="D26" s="2">
         <v>12.7</v>
       </c>
+      <c r="E26" s="9">
+        <v>1207.8</v>
+      </c>
       <c r="F26" s="6" t="s">
         <v>24</v>
       </c>
@@ -5257,8 +5460,12 @@
       <c r="I26" s="7">
         <v>12</v>
       </c>
+      <c r="R26" s="11">
+        <f t="shared" si="0"/>
+        <v>6.2276867030965646E-2</v>
+      </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:18">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -5271,6 +5478,9 @@
       <c r="D27" s="2">
         <v>11.3</v>
       </c>
+      <c r="E27" s="10">
+        <v>1114.2</v>
+      </c>
       <c r="F27" s="1" t="s">
         <v>25</v>
       </c>
@@ -5283,8 +5493,12 @@
       <c r="I27" s="2">
         <v>11</v>
       </c>
+      <c r="R27" s="11">
+        <f t="shared" si="0"/>
+        <v>4.9809728953509082E-2</v>
+      </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:18">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -5297,6 +5511,9 @@
       <c r="D28" s="2">
         <v>8.1999999999999993</v>
       </c>
+      <c r="E28" s="9">
+        <v>1261.8</v>
+      </c>
       <c r="F28" s="1" t="s">
         <v>26</v>
       </c>
@@ -5309,8 +5526,12 @@
       <c r="I28" s="2">
         <v>7</v>
       </c>
+      <c r="R28" s="11">
+        <f t="shared" si="0"/>
+        <v>2.5802028847677936E-2</v>
+      </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:18">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -5323,6 +5544,9 @@
       <c r="D29" s="2">
         <v>7</v>
       </c>
+      <c r="E29" s="10">
+        <v>1092.3</v>
+      </c>
       <c r="F29" s="1" t="s">
         <v>27</v>
       </c>
@@ -5335,8 +5559,12 @@
       <c r="I29" s="2">
         <v>5</v>
       </c>
+      <c r="R29" s="11">
+        <f t="shared" si="0"/>
+        <v>2.7193994323903854E-2</v>
+      </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:18">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -5349,6 +5577,9 @@
       <c r="D30" s="2">
         <v>4.5999999999999996</v>
       </c>
+      <c r="E30" s="9">
+        <v>923.7</v>
+      </c>
       <c r="F30" s="1" t="s">
         <v>28</v>
       </c>
@@ -5361,8 +5592,12 @@
       <c r="I30" s="2">
         <v>4</v>
       </c>
+      <c r="R30" s="11">
+        <f t="shared" si="0"/>
+        <v>3.7337880264155063E-2</v>
+      </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:18">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -5375,6 +5610,9 @@
       <c r="D31" s="2">
         <v>3.7</v>
       </c>
+      <c r="E31" s="10">
+        <v>783.5</v>
+      </c>
       <c r="F31" s="4" t="s">
         <v>29</v>
       </c>
@@ -5390,8 +5628,12 @@
       <c r="J31" t="s">
         <v>44</v>
       </c>
+      <c r="R31" s="11">
+        <f t="shared" si="0"/>
+        <v>3.7027440970006341E-2</v>
+      </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:18">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -5404,6 +5646,9 @@
       <c r="D32" s="2">
         <v>7.1</v>
       </c>
+      <c r="E32" s="9">
+        <v>1154</v>
+      </c>
       <c r="F32" s="1" t="s">
         <v>30</v>
       </c>
@@ -5419,8 +5664,12 @@
       <c r="J32" t="s">
         <v>45</v>
       </c>
+      <c r="R32" s="11">
+        <f t="shared" si="0"/>
+        <v>4.3064991334488836E-2</v>
+      </c>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:18">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -5433,6 +5682,9 @@
       <c r="D33" s="2">
         <v>5.4</v>
       </c>
+      <c r="E33" s="10">
+        <v>1051.0999999999999</v>
+      </c>
       <c r="F33" s="1" t="s">
         <v>31</v>
       </c>
@@ -5445,8 +5697,12 @@
       <c r="I33" s="2">
         <v>5</v>
       </c>
+      <c r="R33" s="11">
+        <f t="shared" si="0"/>
+        <v>5.4070973266102024E-2</v>
+      </c>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:18">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -5459,6 +5715,9 @@
       <c r="D34" s="2">
         <v>5.4</v>
       </c>
+      <c r="E34" s="9">
+        <v>962.9</v>
+      </c>
       <c r="F34" s="1" t="s">
         <v>32</v>
       </c>
@@ -5471,8 +5730,12 @@
       <c r="I34" s="2">
         <v>5</v>
       </c>
+      <c r="R34" s="11">
+        <f t="shared" si="0"/>
+        <v>5.1677225049330255E-2</v>
+      </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:18">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -5485,6 +5748,9 @@
       <c r="D35" s="2">
         <v>3.6</v>
       </c>
+      <c r="E35" s="10">
+        <v>776.1</v>
+      </c>
       <c r="F35" s="4" t="s">
         <v>33</v>
       </c>
@@ -5497,8 +5763,12 @@
       <c r="I35" s="5">
         <v>3</v>
       </c>
+      <c r="R35" s="11">
+        <f t="shared" si="0"/>
+        <v>9.6263368122664644E-2</v>
+      </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:18">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -5524,17 +5794,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:18">
       <c r="A38" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:18">
       <c r="A39" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:18">
       <c r="A40" s="1" t="s">
         <v>48</v>
       </c>

</xml_diff>